<commit_message>
New and changed Documents are finished for the upload
</commit_message>
<xml_diff>
--- a/Testdokumente/Fehlerliste.xlsx
+++ b/Testdokumente/Fehlerliste.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaming Laptop\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/varmahal/Library/Mobile Documents/com~apple~CloudDocs/yourChoice/Documentation/Testdokumente/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F407BEAA-836A-8F47-9A17-0844FC0F3BDC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
   <si>
     <t>Fehlermeldung</t>
   </si>
@@ -182,7 +183,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -326,22 +327,22 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="16" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -349,7 +350,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -365,7 +366,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -660,24 +661,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="116" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="124.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="2"/>
+    <col min="1" max="1" width="18.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="124.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="11.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -703,7 +704,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -727,7 +728,7 @@
       </c>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -745,7 +746,7 @@
       <c r="H3" s="7"/>
       <c r="I3" s="11"/>
     </row>
-    <row r="4" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -763,7 +764,7 @@
       <c r="H4" s="7"/>
       <c r="I4" s="11"/>
     </row>
-    <row r="5" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -781,7 +782,7 @@
       <c r="H5" s="9"/>
       <c r="I5" s="11"/>
     </row>
-    <row r="6" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -799,7 +800,7 @@
       <c r="H6" s="9"/>
       <c r="I6" s="11"/>
     </row>
-    <row r="7" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -813,11 +814,11 @@
         <v>4</v>
       </c>
       <c r="F7" s="13"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="16"/>
-    </row>
-    <row r="8" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="15"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="19"/>
+    </row>
+    <row r="8" spans="1:9" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -830,12 +831,12 @@
       <c r="D8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="19"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="18"/>
       <c r="I8" s="20"/>
     </row>
-    <row r="9" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -849,7 +850,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -863,7 +864,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -877,7 +878,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
@@ -891,7 +892,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -905,7 +906,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -919,7 +920,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -933,7 +934,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -947,7 +948,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -961,71 +962,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
+    <row r="18" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="19" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="20" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="21" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="22" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="G7:G8"/>

</xml_diff>